<commit_message>
codes added into excel write
</commit_message>
<xml_diff>
--- a/src/Book1.xlsx
+++ b/src/Book1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/home/IdeaProjects/Crm24/src/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>firstName</t>
   </si>
@@ -55,12 +55,25 @@
   </si>
   <si>
     <t>Yildiz</t>
+  </si>
+  <si>
+    <t>Hero</t>
+  </si>
+  <si>
+    <t>Okan</t>
+  </si>
+  <si>
+    <t>Ayhan</t>
+  </si>
+  <si>
+    <t>grandma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -430,7 +443,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="20.83203125" customWidth="1"/>
+    <col min="1" max="3" customWidth="true" width="20.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
@@ -446,7 +459,7 @@
     </row>
     <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -468,7 +481,7 @@
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -484,8 +497,8 @@
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2">
-        <v>1546</v>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">

</xml_diff>